<commit_message>
updating the data file
</commit_message>
<xml_diff>
--- a/public/data/data.xlsx
+++ b/public/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/riley45/Documents/Gitlab/weather/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DE9E91-6546-F54A-BE57-4E53CE701748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0E522D-BE9C-354C-BDD1-32E3E365092F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12160" yWindow="12940" windowWidth="43200" windowHeight="23540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Removed" sheetId="9" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">NIF!$A$1:$G$81</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">NIF!$A$1:$F$81</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">NIF!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -1141,7 +1141,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1346,9 +1346,6 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1369,9 +1366,6 @@
     </xf>
     <xf numFmtId="14" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1776,97 +1770,94 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:FL81"/>
+  <dimension ref="A1:FK81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A82" sqref="A82:XFD89"/>
+    <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" style="75" customWidth="1"/>
-    <col min="2" max="2" width="14" style="75" customWidth="1"/>
-    <col min="3" max="3" width="81.6640625" style="76" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="80" customWidth="1"/>
-    <col min="5" max="5" width="12" style="85" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="6" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" style="84" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.6640625" style="3"/>
+    <col min="1" max="1" width="15.6640625" style="74" customWidth="1"/>
+    <col min="2" max="2" width="14" style="74" customWidth="1"/>
+    <col min="3" max="3" width="81.6640625" style="75" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="78" customWidth="1"/>
+    <col min="5" max="5" width="12" style="83" customWidth="1"/>
+    <col min="6" max="6" width="13.5" style="82" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.6640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="16" customFormat="1" ht="76" x14ac:dyDescent="0.2">
-      <c r="A1" s="92">
+    <row r="1" spans="1:21" s="16" customFormat="1" ht="76" x14ac:dyDescent="0.2">
+      <c r="A1" s="90">
         <v>391</v>
       </c>
-      <c r="B1" s="92">
+      <c r="B1" s="90">
         <v>648962</v>
       </c>
-      <c r="C1" s="95" t="s">
+      <c r="C1" s="93" t="s">
         <v>109</v>
       </c>
-      <c r="D1" s="94" t="s">
+      <c r="D1" s="92" t="s">
         <v>89</v>
       </c>
-      <c r="E1" s="93">
+      <c r="E1" s="91">
         <v>45432</v>
       </c>
-      <c r="F1" s="69"/>
-      <c r="G1" s="93">
+      <c r="F1" s="91">
         <v>45436</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="16" customFormat="1" ht="38" x14ac:dyDescent="0.2">
-      <c r="A2" s="73">
+    <row r="2" spans="1:21" s="16" customFormat="1" ht="38" x14ac:dyDescent="0.2">
+      <c r="A2" s="72">
         <v>391</v>
       </c>
-      <c r="B2" s="73">
+      <c r="B2" s="72">
         <v>629573</v>
       </c>
       <c r="C2" s="69" t="s">
         <v>97</v>
       </c>
-      <c r="D2" s="79" t="s">
+      <c r="D2" s="77" t="s">
         <v>89</v>
       </c>
-      <c r="E2" s="90">
+      <c r="E2" s="88">
         <v>45432</v>
       </c>
-      <c r="F2" s="69"/>
-      <c r="G2" s="90">
+      <c r="F2" s="88">
         <v>45436</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="G2" s="11" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="72">
+    <row r="3" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="71">
         <v>490</v>
       </c>
-      <c r="B3" s="72" t="s">
+      <c r="B3" s="71" t="s">
         <v>111</v>
       </c>
       <c r="C3" s="43" t="s">
         <v>130</v>
       </c>
-      <c r="D3" s="72" t="s">
+      <c r="D3" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E3" s="83">
+      <c r="E3" s="81">
         <v>45436</v>
       </c>
-      <c r="F3" s="45"/>
-      <c r="G3" s="83">
+      <c r="F3" s="81">
         <v>45436</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="G3" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
@@ -1880,31 +1871,30 @@
       <c r="S3" s="2"/>
       <c r="T3" s="2"/>
       <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-    </row>
-    <row r="4" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="72">
+    </row>
+    <row r="4" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="71">
         <v>490</v>
       </c>
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="71" t="s">
         <v>112</v>
       </c>
       <c r="C4" s="43" t="s">
         <v>131</v>
       </c>
-      <c r="D4" s="72" t="s">
+      <c r="D4" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="83">
+      <c r="E4" s="81">
         <v>45436</v>
       </c>
-      <c r="F4" s="45"/>
-      <c r="G4" s="83">
+      <c r="F4" s="81">
         <v>45436</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="G4" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H4" s="10"/>
       <c r="I4" s="10"/>
       <c r="J4" s="10"/>
       <c r="K4" s="10"/>
@@ -1918,31 +1908,30 @@
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
       <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-    </row>
-    <row r="5" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="72">
+    </row>
+    <row r="5" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="71">
         <v>490</v>
       </c>
-      <c r="B5" s="72" t="s">
+      <c r="B5" s="71" t="s">
         <v>113</v>
       </c>
       <c r="C5" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="72" t="s">
+      <c r="D5" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E5" s="83">
+      <c r="E5" s="81">
         <v>45436</v>
       </c>
-      <c r="F5" s="45"/>
-      <c r="G5" s="83">
+      <c r="F5" s="81">
         <v>45436</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="G5" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
@@ -1956,31 +1945,30 @@
       <c r="S5" s="2"/>
       <c r="T5" s="2"/>
       <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-    </row>
-    <row r="6" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="72">
+    </row>
+    <row r="6" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="71">
         <v>490</v>
       </c>
-      <c r="B6" s="72" t="s">
+      <c r="B6" s="71" t="s">
         <v>114</v>
       </c>
       <c r="C6" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="D6" s="72" t="s">
+      <c r="D6" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E6" s="83">
+      <c r="E6" s="81">
         <v>45436</v>
       </c>
-      <c r="F6" s="45"/>
-      <c r="G6" s="83">
+      <c r="F6" s="81">
         <v>45436</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="G6" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H6" s="10"/>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
       <c r="K6" s="10"/>
@@ -1994,31 +1982,30 @@
       <c r="S6" s="10"/>
       <c r="T6" s="10"/>
       <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-    </row>
-    <row r="7" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="72">
+    </row>
+    <row r="7" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="71">
         <v>490</v>
       </c>
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="71" t="s">
         <v>115</v>
       </c>
       <c r="C7" s="43" t="s">
         <v>134</v>
       </c>
-      <c r="D7" s="72" t="s">
+      <c r="D7" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E7" s="83">
+      <c r="E7" s="81">
         <v>45436</v>
       </c>
-      <c r="F7" s="45"/>
-      <c r="G7" s="83">
+      <c r="F7" s="81">
         <v>45436</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="G7" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
@@ -2032,31 +2019,30 @@
       <c r="S7" s="2"/>
       <c r="T7" s="2"/>
       <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-    </row>
-    <row r="8" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="72">
+    </row>
+    <row r="8" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="71">
         <v>490</v>
       </c>
-      <c r="B8" s="72" t="s">
+      <c r="B8" s="71" t="s">
         <v>116</v>
       </c>
       <c r="C8" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="D8" s="72" t="s">
+      <c r="D8" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E8" s="83">
+      <c r="E8" s="81">
         <v>45436</v>
       </c>
-      <c r="F8" s="45"/>
-      <c r="G8" s="83">
+      <c r="F8" s="81">
         <v>45436</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="G8" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
       <c r="K8" s="10"/>
@@ -2070,31 +2056,30 @@
       <c r="S8" s="10"/>
       <c r="T8" s="10"/>
       <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-    </row>
-    <row r="9" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="72">
+    </row>
+    <row r="9" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="71">
         <v>490</v>
       </c>
-      <c r="B9" s="72" t="s">
+      <c r="B9" s="71" t="s">
         <v>117</v>
       </c>
       <c r="C9" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="D9" s="72" t="s">
+      <c r="D9" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="83">
+      <c r="E9" s="81">
         <v>45436</v>
       </c>
-      <c r="F9" s="45"/>
-      <c r="G9" s="83">
+      <c r="F9" s="81">
         <v>45436</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="G9" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
@@ -2108,31 +2093,30 @@
       <c r="S9" s="2"/>
       <c r="T9" s="2"/>
       <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-    </row>
-    <row r="10" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="72">
+    </row>
+    <row r="10" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="71">
         <v>490</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="71" t="s">
         <v>118</v>
       </c>
       <c r="C10" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="D10" s="72" t="s">
+      <c r="D10" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="83">
+      <c r="E10" s="81">
         <v>45434</v>
       </c>
-      <c r="F10" s="45"/>
-      <c r="G10" s="83">
+      <c r="F10" s="81">
         <v>45434</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="G10" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H10" s="10"/>
       <c r="I10" s="10"/>
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
@@ -2146,31 +2130,30 @@
       <c r="S10" s="10"/>
       <c r="T10" s="10"/>
       <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
-    </row>
-    <row r="11" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="72">
+    </row>
+    <row r="11" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="71">
         <v>490</v>
       </c>
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="71" t="s">
         <v>119</v>
       </c>
       <c r="C11" s="43" t="s">
         <v>138</v>
       </c>
-      <c r="D11" s="72" t="s">
+      <c r="D11" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="83">
+      <c r="E11" s="81">
         <v>45434</v>
       </c>
-      <c r="F11" s="45"/>
-      <c r="G11" s="83">
+      <c r="F11" s="81">
         <v>45434</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="G11" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H11" s="2"/>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -2184,31 +2167,30 @@
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-    </row>
-    <row r="12" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="72">
+    </row>
+    <row r="12" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="71">
         <v>490</v>
       </c>
-      <c r="B12" s="72" t="s">
+      <c r="B12" s="71" t="s">
         <v>120</v>
       </c>
       <c r="C12" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="D12" s="72" t="s">
+      <c r="D12" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="83">
+      <c r="E12" s="81">
         <v>45435</v>
       </c>
-      <c r="F12" s="45"/>
-      <c r="G12" s="83">
+      <c r="F12" s="81">
         <v>45435</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="G12" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
       <c r="K12" s="10"/>
@@ -2222,31 +2204,30 @@
       <c r="S12" s="10"/>
       <c r="T12" s="10"/>
       <c r="U12" s="10"/>
-      <c r="V12" s="10"/>
-    </row>
-    <row r="13" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="72">
+    </row>
+    <row r="13" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="71">
         <v>490</v>
       </c>
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="71" t="s">
         <v>121</v>
       </c>
       <c r="C13" s="43" t="s">
         <v>140</v>
       </c>
-      <c r="D13" s="72" t="s">
+      <c r="D13" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E13" s="83">
+      <c r="E13" s="81">
         <v>45435</v>
       </c>
-      <c r="F13" s="45"/>
-      <c r="G13" s="83">
+      <c r="F13" s="81">
         <v>45435</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="G13" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -2260,31 +2241,30 @@
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
-      <c r="V13" s="2"/>
-    </row>
-    <row r="14" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="72">
+    </row>
+    <row r="14" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="71">
         <v>490</v>
       </c>
-      <c r="B14" s="72" t="s">
+      <c r="B14" s="71" t="s">
         <v>122</v>
       </c>
       <c r="C14" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="D14" s="72" t="s">
+      <c r="D14" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="83">
+      <c r="E14" s="81">
         <v>45435</v>
       </c>
-      <c r="F14" s="45"/>
-      <c r="G14" s="83">
+      <c r="F14" s="81">
         <v>45435</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="G14" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
@@ -2298,31 +2278,30 @@
       <c r="S14" s="10"/>
       <c r="T14" s="10"/>
       <c r="U14" s="10"/>
-      <c r="V14" s="10"/>
-    </row>
-    <row r="15" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="72">
+    </row>
+    <row r="15" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="71">
         <v>490</v>
       </c>
-      <c r="B15" s="72" t="s">
+      <c r="B15" s="71" t="s">
         <v>123</v>
       </c>
       <c r="C15" s="43" t="s">
         <v>142</v>
       </c>
-      <c r="D15" s="72" t="s">
+      <c r="D15" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="83">
+      <c r="E15" s="81">
         <v>45435</v>
       </c>
-      <c r="F15" s="45"/>
-      <c r="G15" s="83">
+      <c r="F15" s="81">
         <v>45435</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="G15" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -2336,31 +2315,30 @@
       <c r="S15" s="2"/>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
-      <c r="V15" s="2"/>
-    </row>
-    <row r="16" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="72">
+    </row>
+    <row r="16" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="71">
         <v>490</v>
       </c>
-      <c r="B16" s="72" t="s">
+      <c r="B16" s="71" t="s">
         <v>124</v>
       </c>
       <c r="C16" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="D16" s="72" t="s">
+      <c r="D16" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E16" s="83">
+      <c r="E16" s="81">
         <v>45435</v>
       </c>
-      <c r="F16" s="45"/>
-      <c r="G16" s="83">
+      <c r="F16" s="81">
         <v>45435</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="G16" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H16" s="10"/>
       <c r="I16" s="10"/>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
@@ -2374,31 +2352,30 @@
       <c r="S16" s="10"/>
       <c r="T16" s="10"/>
       <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-    </row>
-    <row r="17" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="72">
+    </row>
+    <row r="17" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="71">
         <v>490</v>
       </c>
-      <c r="B17" s="72" t="s">
+      <c r="B17" s="71" t="s">
         <v>125</v>
       </c>
       <c r="C17" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="D17" s="72" t="s">
+      <c r="D17" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E17" s="83">
+      <c r="E17" s="81">
         <v>45435</v>
       </c>
-      <c r="F17" s="45"/>
-      <c r="G17" s="83">
+      <c r="F17" s="81">
         <v>45435</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="G17" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -2412,31 +2389,30 @@
       <c r="S17" s="2"/>
       <c r="T17" s="2"/>
       <c r="U17" s="2"/>
-      <c r="V17" s="2"/>
-    </row>
-    <row r="18" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="72">
+    </row>
+    <row r="18" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="71">
         <v>490</v>
       </c>
-      <c r="B18" s="72" t="s">
+      <c r="B18" s="71" t="s">
         <v>126</v>
       </c>
       <c r="C18" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="D18" s="72" t="s">
+      <c r="D18" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E18" s="83">
+      <c r="E18" s="81">
         <v>45435</v>
       </c>
-      <c r="F18" s="45"/>
-      <c r="G18" s="83">
+      <c r="F18" s="81">
         <v>45435</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="G18" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="10"/>
       <c r="K18" s="10"/>
@@ -2450,31 +2426,30 @@
       <c r="S18" s="10"/>
       <c r="T18" s="10"/>
       <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
-    </row>
-    <row r="19" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="72">
+    </row>
+    <row r="19" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="71">
         <v>490</v>
       </c>
-      <c r="B19" s="72" t="s">
+      <c r="B19" s="71" t="s">
         <v>127</v>
       </c>
       <c r="C19" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="D19" s="72" t="s">
+      <c r="D19" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="83">
+      <c r="E19" s="81">
         <v>45435</v>
       </c>
-      <c r="F19" s="45"/>
-      <c r="G19" s="83">
+      <c r="F19" s="81">
         <v>45435</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="G19" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
@@ -2488,31 +2463,30 @@
       <c r="S19" s="2"/>
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
-      <c r="V19" s="2"/>
-    </row>
-    <row r="20" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="72">
+    </row>
+    <row r="20" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="71">
         <v>490</v>
       </c>
-      <c r="B20" s="72" t="s">
+      <c r="B20" s="71" t="s">
         <v>128</v>
       </c>
       <c r="C20" s="43" t="s">
         <v>147</v>
       </c>
-      <c r="D20" s="72" t="s">
+      <c r="D20" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E20" s="86">
+      <c r="E20" s="84">
         <v>45432</v>
       </c>
-      <c r="F20" s="43"/>
-      <c r="G20" s="83">
+      <c r="F20" s="81">
         <v>45432</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="G20" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H20" s="10"/>
       <c r="I20" s="10"/>
       <c r="J20" s="10"/>
       <c r="K20" s="10"/>
@@ -2526,31 +2500,30 @@
       <c r="S20" s="10"/>
       <c r="T20" s="10"/>
       <c r="U20" s="10"/>
-      <c r="V20" s="10"/>
-    </row>
-    <row r="21" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="72">
+    </row>
+    <row r="21" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="71">
         <v>490</v>
       </c>
-      <c r="B21" s="72" t="s">
+      <c r="B21" s="71" t="s">
         <v>129</v>
       </c>
       <c r="C21" s="43" t="s">
         <v>148</v>
       </c>
-      <c r="D21" s="72" t="s">
+      <c r="D21" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="86">
+      <c r="E21" s="84">
         <v>45432</v>
       </c>
-      <c r="F21" s="43"/>
-      <c r="G21" s="83">
+      <c r="F21" s="81">
         <v>45432</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="G21" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
@@ -2564,33 +2537,30 @@
       <c r="S21" s="2"/>
       <c r="T21" s="2"/>
       <c r="U21" s="2"/>
-      <c r="V21" s="2"/>
-    </row>
-    <row r="22" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="87">
+    </row>
+    <row r="22" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="85">
         <v>571</v>
       </c>
-      <c r="B22" s="88" t="s">
+      <c r="B22" s="86" t="s">
         <v>161</v>
       </c>
-      <c r="C22" s="88" t="s">
+      <c r="C22" s="86" t="s">
         <v>162</v>
       </c>
-      <c r="D22" s="81" t="s">
+      <c r="D22" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E22" s="89">
+      <c r="E22" s="87">
         <v>45432</v>
       </c>
-      <c r="F22" s="88">
-        <v>1</v>
-      </c>
-      <c r="G22" s="91">
+      <c r="F22" s="89">
         <v>45432</v>
       </c>
-      <c r="H22" s="11" t="s">
+      <c r="G22" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H22" s="10"/>
       <c r="I22" s="10"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
@@ -2604,33 +2574,30 @@
       <c r="S22" s="10"/>
       <c r="T22" s="10"/>
       <c r="U22" s="10"/>
-      <c r="V22" s="10"/>
-    </row>
-    <row r="23" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="87">
+    </row>
+    <row r="23" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="85">
         <v>571</v>
       </c>
-      <c r="B23" s="88" t="s">
+      <c r="B23" s="86" t="s">
         <v>164</v>
       </c>
-      <c r="C23" s="88" t="s">
+      <c r="C23" s="86" t="s">
         <v>165</v>
       </c>
-      <c r="D23" s="81" t="s">
+      <c r="D23" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E23" s="89">
+      <c r="E23" s="87">
         <v>45432</v>
       </c>
-      <c r="F23" s="88">
-        <v>1</v>
-      </c>
-      <c r="G23" s="91">
+      <c r="F23" s="89">
         <v>45432</v>
       </c>
-      <c r="H23" s="11" t="s">
+      <c r="G23" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H23" s="10"/>
       <c r="I23" s="10"/>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
@@ -2644,33 +2611,30 @@
       <c r="S23" s="10"/>
       <c r="T23" s="10"/>
       <c r="U23" s="10"/>
-      <c r="V23" s="10"/>
-    </row>
-    <row r="24" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="87">
+    </row>
+    <row r="24" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="85">
         <v>571</v>
       </c>
-      <c r="B24" s="88" t="s">
+      <c r="B24" s="86" t="s">
         <v>166</v>
       </c>
-      <c r="C24" s="88" t="s">
+      <c r="C24" s="86" t="s">
         <v>167</v>
       </c>
-      <c r="D24" s="81" t="s">
+      <c r="D24" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E24" s="89">
+      <c r="E24" s="87">
         <v>45432</v>
       </c>
-      <c r="F24" s="88">
-        <v>1</v>
-      </c>
-      <c r="G24" s="91">
+      <c r="F24" s="89">
         <v>45432</v>
       </c>
-      <c r="H24" s="11" t="s">
+      <c r="G24" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H24" s="10"/>
       <c r="I24" s="10"/>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
@@ -2684,33 +2648,30 @@
       <c r="S24" s="10"/>
       <c r="T24" s="10"/>
       <c r="U24" s="10"/>
-      <c r="V24" s="10"/>
-    </row>
-    <row r="25" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="87">
+    </row>
+    <row r="25" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="85">
         <v>571</v>
       </c>
-      <c r="B25" s="88" t="s">
+      <c r="B25" s="86" t="s">
         <v>168</v>
       </c>
-      <c r="C25" s="88" t="s">
+      <c r="C25" s="86" t="s">
         <v>169</v>
       </c>
-      <c r="D25" s="81" t="s">
+      <c r="D25" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E25" s="89">
+      <c r="E25" s="87">
         <v>45432</v>
       </c>
-      <c r="F25" s="88">
-        <v>1</v>
-      </c>
-      <c r="G25" s="91">
+      <c r="F25" s="89">
         <v>45432</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="G25" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H25" s="10"/>
       <c r="I25" s="10"/>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -2724,33 +2685,30 @@
       <c r="S25" s="10"/>
       <c r="T25" s="10"/>
       <c r="U25" s="10"/>
-      <c r="V25" s="10"/>
-    </row>
-    <row r="26" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="87">
+    </row>
+    <row r="26" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="85">
         <v>571</v>
       </c>
-      <c r="B26" s="88" t="s">
+      <c r="B26" s="86" t="s">
         <v>170</v>
       </c>
-      <c r="C26" s="88" t="s">
+      <c r="C26" s="86" t="s">
         <v>171</v>
       </c>
-      <c r="D26" s="81" t="s">
+      <c r="D26" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E26" s="89">
+      <c r="E26" s="87">
         <v>45432</v>
       </c>
-      <c r="F26" s="88">
-        <v>1</v>
-      </c>
-      <c r="G26" s="91">
+      <c r="F26" s="89">
         <v>45432</v>
       </c>
-      <c r="H26" s="11" t="s">
+      <c r="G26" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H26" s="10"/>
       <c r="I26" s="10"/>
       <c r="J26" s="10"/>
       <c r="K26" s="10"/>
@@ -2764,33 +2722,30 @@
       <c r="S26" s="10"/>
       <c r="T26" s="10"/>
       <c r="U26" s="10"/>
-      <c r="V26" s="10"/>
-    </row>
-    <row r="27" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="87">
+    </row>
+    <row r="27" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="85">
         <v>571</v>
       </c>
-      <c r="B27" s="88" t="s">
+      <c r="B27" s="86" t="s">
         <v>172</v>
       </c>
-      <c r="C27" s="88" t="s">
+      <c r="C27" s="86" t="s">
         <v>173</v>
       </c>
-      <c r="D27" s="81" t="s">
+      <c r="D27" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E27" s="89">
+      <c r="E27" s="87">
         <v>45432</v>
       </c>
-      <c r="F27" s="88">
-        <v>1</v>
-      </c>
-      <c r="G27" s="91">
+      <c r="F27" s="89">
         <v>45432</v>
       </c>
-      <c r="H27" s="11" t="s">
+      <c r="G27" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H27" s="10"/>
       <c r="I27" s="10"/>
       <c r="J27" s="10"/>
       <c r="K27" s="10"/>
@@ -2804,33 +2759,30 @@
       <c r="S27" s="10"/>
       <c r="T27" s="10"/>
       <c r="U27" s="10"/>
-      <c r="V27" s="10"/>
-    </row>
-    <row r="28" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="87">
+    </row>
+    <row r="28" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="85">
         <v>571</v>
       </c>
-      <c r="B28" s="88" t="s">
+      <c r="B28" s="86" t="s">
         <v>174</v>
       </c>
-      <c r="C28" s="88" t="s">
+      <c r="C28" s="86" t="s">
         <v>175</v>
       </c>
-      <c r="D28" s="81" t="s">
+      <c r="D28" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E28" s="89">
+      <c r="E28" s="87">
         <v>45432</v>
       </c>
-      <c r="F28" s="88">
-        <v>1</v>
-      </c>
-      <c r="G28" s="91">
+      <c r="F28" s="89">
         <v>45432</v>
       </c>
-      <c r="H28" s="11" t="s">
+      <c r="G28" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H28" s="10"/>
       <c r="I28" s="10"/>
       <c r="J28" s="10"/>
       <c r="K28" s="10"/>
@@ -2844,33 +2796,30 @@
       <c r="S28" s="10"/>
       <c r="T28" s="10"/>
       <c r="U28" s="10"/>
-      <c r="V28" s="10"/>
-    </row>
-    <row r="29" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="87">
+    </row>
+    <row r="29" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="85">
         <v>571</v>
       </c>
-      <c r="B29" s="88" t="s">
+      <c r="B29" s="86" t="s">
         <v>176</v>
       </c>
-      <c r="C29" s="88" t="s">
+      <c r="C29" s="86" t="s">
         <v>177</v>
       </c>
-      <c r="D29" s="81" t="s">
+      <c r="D29" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E29" s="89">
+      <c r="E29" s="87">
         <v>45433</v>
       </c>
-      <c r="F29" s="88">
-        <v>1</v>
-      </c>
-      <c r="G29" s="91">
+      <c r="F29" s="89">
         <v>45433</v>
       </c>
-      <c r="H29" s="11" t="s">
+      <c r="G29" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H29" s="10"/>
       <c r="I29" s="10"/>
       <c r="J29" s="10"/>
       <c r="K29" s="10"/>
@@ -2884,33 +2833,30 @@
       <c r="S29" s="10"/>
       <c r="T29" s="10"/>
       <c r="U29" s="10"/>
-      <c r="V29" s="10"/>
-    </row>
-    <row r="30" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="87">
+    </row>
+    <row r="30" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="85">
         <v>571</v>
       </c>
-      <c r="B30" s="88" t="s">
+      <c r="B30" s="86" t="s">
         <v>178</v>
       </c>
-      <c r="C30" s="88" t="s">
+      <c r="C30" s="86" t="s">
         <v>179</v>
       </c>
-      <c r="D30" s="81" t="s">
+      <c r="D30" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E30" s="89">
+      <c r="E30" s="87">
         <v>45433</v>
       </c>
-      <c r="F30" s="88">
-        <v>1</v>
-      </c>
-      <c r="G30" s="91">
+      <c r="F30" s="89">
         <v>45433</v>
       </c>
-      <c r="H30" s="11" t="s">
+      <c r="G30" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H30" s="10"/>
       <c r="I30" s="10"/>
       <c r="J30" s="10"/>
       <c r="K30" s="10"/>
@@ -2924,33 +2870,30 @@
       <c r="S30" s="10"/>
       <c r="T30" s="10"/>
       <c r="U30" s="10"/>
-      <c r="V30" s="10"/>
-    </row>
-    <row r="31" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="87">
+    </row>
+    <row r="31" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="85">
         <v>571</v>
       </c>
-      <c r="B31" s="88" t="s">
+      <c r="B31" s="86" t="s">
         <v>180</v>
       </c>
-      <c r="C31" s="88" t="s">
+      <c r="C31" s="86" t="s">
         <v>181</v>
       </c>
-      <c r="D31" s="81" t="s">
+      <c r="D31" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E31" s="89">
+      <c r="E31" s="87">
         <v>45433</v>
       </c>
-      <c r="F31" s="88">
-        <v>1</v>
-      </c>
-      <c r="G31" s="91">
+      <c r="F31" s="89">
         <v>45433</v>
       </c>
-      <c r="H31" s="11" t="s">
+      <c r="G31" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H31" s="10"/>
       <c r="I31" s="10"/>
       <c r="J31" s="10"/>
       <c r="K31" s="10"/>
@@ -2964,33 +2907,30 @@
       <c r="S31" s="10"/>
       <c r="T31" s="10"/>
       <c r="U31" s="10"/>
-      <c r="V31" s="10"/>
-    </row>
-    <row r="32" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="87">
+    </row>
+    <row r="32" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="85">
         <v>571</v>
       </c>
-      <c r="B32" s="88" t="s">
+      <c r="B32" s="86" t="s">
         <v>182</v>
       </c>
-      <c r="C32" s="88" t="s">
+      <c r="C32" s="86" t="s">
         <v>183</v>
       </c>
-      <c r="D32" s="81" t="s">
+      <c r="D32" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E32" s="89">
+      <c r="E32" s="87">
         <v>45433</v>
       </c>
-      <c r="F32" s="88">
-        <v>1</v>
-      </c>
-      <c r="G32" s="91">
+      <c r="F32" s="89">
         <v>45433</v>
       </c>
-      <c r="H32" s="11" t="s">
+      <c r="G32" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H32" s="10"/>
       <c r="I32" s="10"/>
       <c r="J32" s="10"/>
       <c r="K32" s="10"/>
@@ -3004,33 +2944,30 @@
       <c r="S32" s="10"/>
       <c r="T32" s="10"/>
       <c r="U32" s="10"/>
-      <c r="V32" s="10"/>
-    </row>
-    <row r="33" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="87">
+    </row>
+    <row r="33" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="85">
         <v>571</v>
       </c>
-      <c r="B33" s="88" t="s">
+      <c r="B33" s="86" t="s">
         <v>184</v>
       </c>
-      <c r="C33" s="88" t="s">
+      <c r="C33" s="86" t="s">
         <v>185</v>
       </c>
-      <c r="D33" s="81" t="s">
+      <c r="D33" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E33" s="89">
+      <c r="E33" s="87">
         <v>45433</v>
       </c>
-      <c r="F33" s="88">
-        <v>1</v>
-      </c>
-      <c r="G33" s="91">
+      <c r="F33" s="89">
         <v>45433</v>
       </c>
-      <c r="H33" s="11" t="s">
+      <c r="G33" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H33" s="10"/>
       <c r="I33" s="10"/>
       <c r="J33" s="10"/>
       <c r="K33" s="10"/>
@@ -3044,33 +2981,30 @@
       <c r="S33" s="10"/>
       <c r="T33" s="10"/>
       <c r="U33" s="10"/>
-      <c r="V33" s="10"/>
-    </row>
-    <row r="34" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="87">
+    </row>
+    <row r="34" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="85">
         <v>571</v>
       </c>
-      <c r="B34" s="88" t="s">
+      <c r="B34" s="86" t="s">
         <v>186</v>
       </c>
-      <c r="C34" s="88" t="s">
+      <c r="C34" s="86" t="s">
         <v>187</v>
       </c>
-      <c r="D34" s="81" t="s">
+      <c r="D34" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E34" s="89">
+      <c r="E34" s="87">
         <v>45433</v>
       </c>
-      <c r="F34" s="88">
-        <v>1</v>
-      </c>
-      <c r="G34" s="91">
+      <c r="F34" s="89">
         <v>45433</v>
       </c>
-      <c r="H34" s="11" t="s">
+      <c r="G34" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H34" s="10"/>
       <c r="I34" s="10"/>
       <c r="J34" s="10"/>
       <c r="K34" s="10"/>
@@ -3084,33 +3018,30 @@
       <c r="S34" s="10"/>
       <c r="T34" s="10"/>
       <c r="U34" s="10"/>
-      <c r="V34" s="10"/>
-    </row>
-    <row r="35" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="87">
+    </row>
+    <row r="35" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="85">
         <v>571</v>
       </c>
-      <c r="B35" s="88" t="s">
+      <c r="B35" s="86" t="s">
         <v>188</v>
       </c>
-      <c r="C35" s="88" t="s">
+      <c r="C35" s="86" t="s">
         <v>189</v>
       </c>
-      <c r="D35" s="81" t="s">
+      <c r="D35" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E35" s="89">
+      <c r="E35" s="87">
         <v>45433</v>
       </c>
-      <c r="F35" s="88">
-        <v>1</v>
-      </c>
-      <c r="G35" s="91">
+      <c r="F35" s="89">
         <v>45433</v>
       </c>
-      <c r="H35" s="11" t="s">
+      <c r="G35" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H35" s="10"/>
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
       <c r="K35" s="10"/>
@@ -3124,33 +3055,30 @@
       <c r="S35" s="10"/>
       <c r="T35" s="10"/>
       <c r="U35" s="10"/>
-      <c r="V35" s="10"/>
-    </row>
-    <row r="36" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="87">
+    </row>
+    <row r="36" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="85">
         <v>571</v>
       </c>
-      <c r="B36" s="88" t="s">
+      <c r="B36" s="86" t="s">
         <v>190</v>
       </c>
-      <c r="C36" s="88" t="s">
+      <c r="C36" s="86" t="s">
         <v>191</v>
       </c>
-      <c r="D36" s="81" t="s">
+      <c r="D36" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E36" s="89">
+      <c r="E36" s="87">
         <v>45434</v>
       </c>
-      <c r="F36" s="88">
-        <v>1</v>
-      </c>
-      <c r="G36" s="91">
+      <c r="F36" s="89">
         <v>45434</v>
       </c>
-      <c r="H36" s="11" t="s">
+      <c r="G36" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H36" s="10"/>
       <c r="I36" s="10"/>
       <c r="J36" s="10"/>
       <c r="K36" s="10"/>
@@ -3164,33 +3092,30 @@
       <c r="S36" s="10"/>
       <c r="T36" s="10"/>
       <c r="U36" s="10"/>
-      <c r="V36" s="10"/>
-    </row>
-    <row r="37" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="87">
+    </row>
+    <row r="37" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="85">
         <v>571</v>
       </c>
-      <c r="B37" s="88" t="s">
+      <c r="B37" s="86" t="s">
         <v>192</v>
       </c>
-      <c r="C37" s="88" t="s">
+      <c r="C37" s="86" t="s">
         <v>193</v>
       </c>
-      <c r="D37" s="81" t="s">
+      <c r="D37" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E37" s="89">
+      <c r="E37" s="87">
         <v>45434</v>
       </c>
-      <c r="F37" s="88">
-        <v>1</v>
-      </c>
-      <c r="G37" s="91">
+      <c r="F37" s="89">
         <v>45434</v>
       </c>
-      <c r="H37" s="11" t="s">
+      <c r="G37" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H37" s="10"/>
       <c r="I37" s="10"/>
       <c r="J37" s="10"/>
       <c r="K37" s="10"/>
@@ -3204,33 +3129,30 @@
       <c r="S37" s="10"/>
       <c r="T37" s="10"/>
       <c r="U37" s="10"/>
-      <c r="V37" s="10"/>
-    </row>
-    <row r="38" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="87">
+    </row>
+    <row r="38" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="85">
         <v>571</v>
       </c>
-      <c r="B38" s="88" t="s">
+      <c r="B38" s="86" t="s">
         <v>194</v>
       </c>
-      <c r="C38" s="88" t="s">
+      <c r="C38" s="86" t="s">
         <v>195</v>
       </c>
-      <c r="D38" s="81" t="s">
+      <c r="D38" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E38" s="89">
+      <c r="E38" s="87">
         <v>45434</v>
       </c>
-      <c r="F38" s="88">
-        <v>1</v>
-      </c>
-      <c r="G38" s="91">
+      <c r="F38" s="89">
         <v>45434</v>
       </c>
-      <c r="H38" s="11" t="s">
+      <c r="G38" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H38" s="10"/>
       <c r="I38" s="10"/>
       <c r="J38" s="10"/>
       <c r="K38" s="10"/>
@@ -3244,33 +3166,30 @@
       <c r="S38" s="10"/>
       <c r="T38" s="10"/>
       <c r="U38" s="10"/>
-      <c r="V38" s="10"/>
-    </row>
-    <row r="39" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="87">
+    </row>
+    <row r="39" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="85">
         <v>571</v>
       </c>
-      <c r="B39" s="88" t="s">
+      <c r="B39" s="86" t="s">
         <v>196</v>
       </c>
-      <c r="C39" s="88" t="s">
+      <c r="C39" s="86" t="s">
         <v>197</v>
       </c>
-      <c r="D39" s="81" t="s">
+      <c r="D39" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E39" s="89">
+      <c r="E39" s="87">
         <v>45434</v>
       </c>
-      <c r="F39" s="88">
-        <v>1</v>
-      </c>
-      <c r="G39" s="91">
+      <c r="F39" s="89">
         <v>45434</v>
       </c>
-      <c r="H39" s="11" t="s">
+      <c r="G39" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H39" s="10"/>
       <c r="I39" s="10"/>
       <c r="J39" s="10"/>
       <c r="K39" s="10"/>
@@ -3284,33 +3203,30 @@
       <c r="S39" s="10"/>
       <c r="T39" s="10"/>
       <c r="U39" s="10"/>
-      <c r="V39" s="10"/>
-    </row>
-    <row r="40" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="87">
+    </row>
+    <row r="40" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="85">
         <v>571</v>
       </c>
-      <c r="B40" s="88" t="s">
+      <c r="B40" s="86" t="s">
         <v>198</v>
       </c>
-      <c r="C40" s="88" t="s">
+      <c r="C40" s="86" t="s">
         <v>199</v>
       </c>
-      <c r="D40" s="81" t="s">
+      <c r="D40" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E40" s="89">
+      <c r="E40" s="87">
         <v>45434</v>
       </c>
-      <c r="F40" s="88">
-        <v>1</v>
-      </c>
-      <c r="G40" s="91">
+      <c r="F40" s="89">
         <v>45434</v>
       </c>
-      <c r="H40" s="11" t="s">
+      <c r="G40" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H40" s="10"/>
       <c r="I40" s="10"/>
       <c r="J40" s="10"/>
       <c r="K40" s="10"/>
@@ -3324,33 +3240,30 @@
       <c r="S40" s="10"/>
       <c r="T40" s="10"/>
       <c r="U40" s="10"/>
-      <c r="V40" s="10"/>
-    </row>
-    <row r="41" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="87">
+    </row>
+    <row r="41" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="85">
         <v>571</v>
       </c>
-      <c r="B41" s="88" t="s">
+      <c r="B41" s="86" t="s">
         <v>200</v>
       </c>
-      <c r="C41" s="88" t="s">
+      <c r="C41" s="86" t="s">
         <v>201</v>
       </c>
-      <c r="D41" s="81" t="s">
+      <c r="D41" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E41" s="89">
+      <c r="E41" s="87">
         <v>45434</v>
       </c>
-      <c r="F41" s="88">
-        <v>1</v>
-      </c>
-      <c r="G41" s="91">
+      <c r="F41" s="89">
         <v>45434</v>
       </c>
-      <c r="H41" s="11" t="s">
+      <c r="G41" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H41" s="10"/>
       <c r="I41" s="10"/>
       <c r="J41" s="10"/>
       <c r="K41" s="10"/>
@@ -3364,33 +3277,30 @@
       <c r="S41" s="10"/>
       <c r="T41" s="10"/>
       <c r="U41" s="10"/>
-      <c r="V41" s="10"/>
-    </row>
-    <row r="42" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="87">
+    </row>
+    <row r="42" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="85">
         <v>571</v>
       </c>
-      <c r="B42" s="88" t="s">
+      <c r="B42" s="86" t="s">
         <v>202</v>
       </c>
-      <c r="C42" s="88" t="s">
+      <c r="C42" s="86" t="s">
         <v>203</v>
       </c>
-      <c r="D42" s="81" t="s">
+      <c r="D42" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E42" s="89">
+      <c r="E42" s="87">
         <v>45434</v>
       </c>
-      <c r="F42" s="88">
-        <v>1</v>
-      </c>
-      <c r="G42" s="91">
+      <c r="F42" s="89">
         <v>45434</v>
       </c>
-      <c r="H42" s="11" t="s">
+      <c r="G42" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H42" s="10"/>
       <c r="I42" s="10"/>
       <c r="J42" s="10"/>
       <c r="K42" s="10"/>
@@ -3404,33 +3314,30 @@
       <c r="S42" s="10"/>
       <c r="T42" s="10"/>
       <c r="U42" s="10"/>
-      <c r="V42" s="10"/>
-    </row>
-    <row r="43" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="87">
+    </row>
+    <row r="43" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="85">
         <v>571</v>
       </c>
-      <c r="B43" s="88" t="s">
+      <c r="B43" s="86" t="s">
         <v>204</v>
       </c>
-      <c r="C43" s="88" t="s">
+      <c r="C43" s="86" t="s">
         <v>205</v>
       </c>
-      <c r="D43" s="81" t="s">
+      <c r="D43" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E43" s="89">
+      <c r="E43" s="87">
         <v>45434</v>
       </c>
-      <c r="F43" s="88">
-        <v>1</v>
-      </c>
-      <c r="G43" s="91">
+      <c r="F43" s="89">
         <v>45434</v>
       </c>
-      <c r="H43" s="11" t="s">
+      <c r="G43" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H43" s="10"/>
       <c r="I43" s="10"/>
       <c r="J43" s="10"/>
       <c r="K43" s="10"/>
@@ -3444,33 +3351,30 @@
       <c r="S43" s="10"/>
       <c r="T43" s="10"/>
       <c r="U43" s="10"/>
-      <c r="V43" s="10"/>
-    </row>
-    <row r="44" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="87">
+    </row>
+    <row r="44" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="85">
         <v>571</v>
       </c>
-      <c r="B44" s="88" t="s">
+      <c r="B44" s="86" t="s">
         <v>206</v>
       </c>
-      <c r="C44" s="88" t="s">
+      <c r="C44" s="86" t="s">
         <v>207</v>
       </c>
-      <c r="D44" s="81" t="s">
+      <c r="D44" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E44" s="89">
+      <c r="E44" s="87">
         <v>45435</v>
       </c>
-      <c r="F44" s="88">
-        <v>1</v>
-      </c>
-      <c r="G44" s="91">
+      <c r="F44" s="89">
         <v>45435</v>
       </c>
-      <c r="H44" s="11" t="s">
+      <c r="G44" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H44" s="10"/>
       <c r="I44" s="10"/>
       <c r="J44" s="10"/>
       <c r="K44" s="10"/>
@@ -3484,33 +3388,30 @@
       <c r="S44" s="10"/>
       <c r="T44" s="10"/>
       <c r="U44" s="10"/>
-      <c r="V44" s="10"/>
-    </row>
-    <row r="45" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="87">
+    </row>
+    <row r="45" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="85">
         <v>571</v>
       </c>
-      <c r="B45" s="88" t="s">
+      <c r="B45" s="86" t="s">
         <v>208</v>
       </c>
-      <c r="C45" s="88" t="s">
+      <c r="C45" s="86" t="s">
         <v>209</v>
       </c>
-      <c r="D45" s="81" t="s">
+      <c r="D45" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E45" s="89">
+      <c r="E45" s="87">
         <v>45435</v>
       </c>
-      <c r="F45" s="88">
-        <v>1</v>
-      </c>
-      <c r="G45" s="91">
+      <c r="F45" s="89">
         <v>45435</v>
       </c>
-      <c r="H45" s="11" t="s">
+      <c r="G45" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H45" s="10"/>
       <c r="I45" s="10"/>
       <c r="J45" s="10"/>
       <c r="K45" s="10"/>
@@ -3524,33 +3425,30 @@
       <c r="S45" s="10"/>
       <c r="T45" s="10"/>
       <c r="U45" s="10"/>
-      <c r="V45" s="10"/>
-    </row>
-    <row r="46" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="87">
+    </row>
+    <row r="46" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="85">
         <v>571</v>
       </c>
-      <c r="B46" s="88" t="s">
+      <c r="B46" s="86" t="s">
         <v>210</v>
       </c>
-      <c r="C46" s="88" t="s">
+      <c r="C46" s="86" t="s">
         <v>211</v>
       </c>
-      <c r="D46" s="81" t="s">
+      <c r="D46" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E46" s="89">
+      <c r="E46" s="87">
         <v>45435</v>
       </c>
-      <c r="F46" s="88">
-        <v>1</v>
-      </c>
-      <c r="G46" s="91">
+      <c r="F46" s="89">
         <v>45435</v>
       </c>
-      <c r="H46" s="11" t="s">
+      <c r="G46" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H46" s="10"/>
       <c r="I46" s="10"/>
       <c r="J46" s="10"/>
       <c r="K46" s="10"/>
@@ -3564,33 +3462,30 @@
       <c r="S46" s="10"/>
       <c r="T46" s="10"/>
       <c r="U46" s="10"/>
-      <c r="V46" s="10"/>
-    </row>
-    <row r="47" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="87">
+    </row>
+    <row r="47" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="85">
         <v>571</v>
       </c>
-      <c r="B47" s="88" t="s">
+      <c r="B47" s="86" t="s">
         <v>212</v>
       </c>
-      <c r="C47" s="88" t="s">
+      <c r="C47" s="86" t="s">
         <v>213</v>
       </c>
-      <c r="D47" s="81" t="s">
+      <c r="D47" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E47" s="89">
+      <c r="E47" s="87">
         <v>45435</v>
       </c>
-      <c r="F47" s="88">
-        <v>1</v>
-      </c>
-      <c r="G47" s="91">
+      <c r="F47" s="89">
         <v>45435</v>
       </c>
-      <c r="H47" s="11" t="s">
+      <c r="G47" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H47" s="10"/>
       <c r="I47" s="10"/>
       <c r="J47" s="10"/>
       <c r="K47" s="10"/>
@@ -3604,33 +3499,30 @@
       <c r="S47" s="10"/>
       <c r="T47" s="10"/>
       <c r="U47" s="10"/>
-      <c r="V47" s="10"/>
-    </row>
-    <row r="48" spans="1:22" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="87">
+    </row>
+    <row r="48" spans="1:21" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="85">
         <v>571</v>
       </c>
-      <c r="B48" s="88" t="s">
+      <c r="B48" s="86" t="s">
         <v>214</v>
       </c>
-      <c r="C48" s="88" t="s">
+      <c r="C48" s="86" t="s">
         <v>215</v>
       </c>
-      <c r="D48" s="81" t="s">
+      <c r="D48" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E48" s="89">
+      <c r="E48" s="87">
         <v>45435</v>
       </c>
-      <c r="F48" s="88">
-        <v>1</v>
-      </c>
-      <c r="G48" s="91">
+      <c r="F48" s="89">
         <v>45435</v>
       </c>
-      <c r="H48" s="11" t="s">
+      <c r="G48" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H48" s="10"/>
       <c r="I48" s="10"/>
       <c r="J48" s="10"/>
       <c r="K48" s="10"/>
@@ -3644,33 +3536,30 @@
       <c r="S48" s="10"/>
       <c r="T48" s="10"/>
       <c r="U48" s="10"/>
-      <c r="V48" s="10"/>
-    </row>
-    <row r="49" spans="1:168" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="87">
+    </row>
+    <row r="49" spans="1:167" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="85">
         <v>571</v>
       </c>
-      <c r="B49" s="88" t="s">
+      <c r="B49" s="86" t="s">
         <v>216</v>
       </c>
-      <c r="C49" s="88" t="s">
+      <c r="C49" s="86" t="s">
         <v>217</v>
       </c>
-      <c r="D49" s="81" t="s">
+      <c r="D49" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E49" s="89">
+      <c r="E49" s="87">
         <v>45435</v>
       </c>
-      <c r="F49" s="88">
-        <v>1</v>
-      </c>
-      <c r="G49" s="91">
+      <c r="F49" s="89">
         <v>45435</v>
       </c>
-      <c r="H49" s="11" t="s">
+      <c r="G49" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H49" s="10"/>
       <c r="I49" s="10"/>
       <c r="J49" s="10"/>
       <c r="K49" s="10"/>
@@ -3684,33 +3573,30 @@
       <c r="S49" s="10"/>
       <c r="T49" s="10"/>
       <c r="U49" s="10"/>
-      <c r="V49" s="10"/>
-    </row>
-    <row r="50" spans="1:168" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="87">
+    </row>
+    <row r="50" spans="1:167" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="85">
         <v>571</v>
       </c>
-      <c r="B50" s="88" t="s">
+      <c r="B50" s="86" t="s">
         <v>218</v>
       </c>
-      <c r="C50" s="88" t="s">
+      <c r="C50" s="86" t="s">
         <v>219</v>
       </c>
-      <c r="D50" s="81" t="s">
+      <c r="D50" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E50" s="89">
+      <c r="E50" s="87">
         <v>45435</v>
       </c>
-      <c r="F50" s="88">
-        <v>1</v>
-      </c>
-      <c r="G50" s="91">
+      <c r="F50" s="89">
         <v>45435</v>
       </c>
-      <c r="H50" s="11" t="s">
+      <c r="G50" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H50" s="10"/>
       <c r="I50" s="10"/>
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
@@ -3724,33 +3610,30 @@
       <c r="S50" s="10"/>
       <c r="T50" s="10"/>
       <c r="U50" s="10"/>
-      <c r="V50" s="10"/>
-    </row>
-    <row r="51" spans="1:168" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="87">
+    </row>
+    <row r="51" spans="1:167" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="85">
         <v>571</v>
       </c>
-      <c r="B51" s="88" t="s">
+      <c r="B51" s="86" t="s">
         <v>220</v>
       </c>
-      <c r="C51" s="88" t="s">
+      <c r="C51" s="86" t="s">
         <v>221</v>
       </c>
-      <c r="D51" s="81" t="s">
+      <c r="D51" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E51" s="89">
+      <c r="E51" s="87">
         <v>45435</v>
       </c>
-      <c r="F51" s="88">
-        <v>1</v>
-      </c>
-      <c r="G51" s="89">
+      <c r="F51" s="87">
         <v>45435</v>
       </c>
-      <c r="H51" s="11" t="s">
+      <c r="G51" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H51" s="10"/>
       <c r="I51" s="10"/>
       <c r="J51" s="10"/>
       <c r="K51" s="10"/>
@@ -3764,33 +3647,30 @@
       <c r="S51" s="10"/>
       <c r="T51" s="10"/>
       <c r="U51" s="10"/>
-      <c r="V51" s="10"/>
-    </row>
-    <row r="52" spans="1:168" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="87">
+    </row>
+    <row r="52" spans="1:167" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="85">
         <v>571</v>
       </c>
-      <c r="B52" s="88" t="s">
+      <c r="B52" s="86" t="s">
         <v>222</v>
       </c>
-      <c r="C52" s="88" t="s">
+      <c r="C52" s="86" t="s">
         <v>223</v>
       </c>
-      <c r="D52" s="81" t="s">
+      <c r="D52" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E52" s="89">
+      <c r="E52" s="87">
         <v>45435</v>
       </c>
-      <c r="F52" s="88">
-        <v>1</v>
-      </c>
-      <c r="G52" s="89">
+      <c r="F52" s="87">
         <v>45435</v>
       </c>
-      <c r="H52" s="11" t="s">
+      <c r="G52" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H52" s="2"/>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
@@ -3804,33 +3684,30 @@
       <c r="S52" s="2"/>
       <c r="T52" s="2"/>
       <c r="U52" s="2"/>
-      <c r="V52" s="2"/>
-    </row>
-    <row r="53" spans="1:168" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="87">
+    </row>
+    <row r="53" spans="1:167" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="85">
         <v>571</v>
       </c>
-      <c r="B53" s="88" t="s">
+      <c r="B53" s="86" t="s">
         <v>224</v>
       </c>
-      <c r="C53" s="88" t="s">
+      <c r="C53" s="86" t="s">
         <v>225</v>
       </c>
-      <c r="D53" s="81" t="s">
+      <c r="D53" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E53" s="89">
+      <c r="E53" s="87">
         <v>45436</v>
       </c>
-      <c r="F53" s="88">
-        <v>1</v>
-      </c>
-      <c r="G53" s="91">
+      <c r="F53" s="89">
         <v>45436</v>
       </c>
-      <c r="H53" s="11" t="s">
+      <c r="G53" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H53" s="10"/>
       <c r="I53" s="10"/>
       <c r="J53" s="10"/>
       <c r="K53" s="10"/>
@@ -3844,33 +3721,30 @@
       <c r="S53" s="10"/>
       <c r="T53" s="10"/>
       <c r="U53" s="10"/>
-      <c r="V53" s="10"/>
-    </row>
-    <row r="54" spans="1:168" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="87">
+    </row>
+    <row r="54" spans="1:167" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="85">
         <v>571</v>
       </c>
-      <c r="B54" s="88" t="s">
+      <c r="B54" s="86" t="s">
         <v>226</v>
       </c>
-      <c r="C54" s="88" t="s">
+      <c r="C54" s="86" t="s">
         <v>227</v>
       </c>
-      <c r="D54" s="81" t="s">
+      <c r="D54" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E54" s="89">
+      <c r="E54" s="87">
         <v>45436</v>
       </c>
-      <c r="F54" s="88">
-        <v>1</v>
-      </c>
-      <c r="G54" s="91">
+      <c r="F54" s="89">
         <v>45436</v>
       </c>
-      <c r="H54" s="11" t="s">
+      <c r="G54" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H54" s="2"/>
       <c r="I54" s="2"/>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
@@ -3884,33 +3758,30 @@
       <c r="S54" s="2"/>
       <c r="T54" s="2"/>
       <c r="U54" s="2"/>
-      <c r="V54" s="2"/>
-    </row>
-    <row r="55" spans="1:168" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="87">
+    </row>
+    <row r="55" spans="1:167" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="85">
         <v>571</v>
       </c>
-      <c r="B55" s="88" t="s">
+      <c r="B55" s="86" t="s">
         <v>228</v>
       </c>
-      <c r="C55" s="88" t="s">
+      <c r="C55" s="86" t="s">
         <v>229</v>
       </c>
-      <c r="D55" s="81" t="s">
+      <c r="D55" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E55" s="89">
+      <c r="E55" s="87">
         <v>45436</v>
       </c>
-      <c r="F55" s="88">
-        <v>1</v>
-      </c>
-      <c r="G55" s="91">
+      <c r="F55" s="89">
         <v>45436</v>
       </c>
-      <c r="H55" s="11" t="s">
+      <c r="G55" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H55" s="10"/>
       <c r="I55" s="10"/>
       <c r="J55" s="10"/>
       <c r="K55" s="10"/>
@@ -3924,33 +3795,30 @@
       <c r="S55" s="10"/>
       <c r="T55" s="10"/>
       <c r="U55" s="10"/>
-      <c r="V55" s="10"/>
-    </row>
-    <row r="56" spans="1:168" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="87">
+    </row>
+    <row r="56" spans="1:167" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="85">
         <v>571</v>
       </c>
-      <c r="B56" s="88" t="s">
+      <c r="B56" s="86" t="s">
         <v>230</v>
       </c>
-      <c r="C56" s="88" t="s">
+      <c r="C56" s="86" t="s">
         <v>231</v>
       </c>
-      <c r="D56" s="81" t="s">
+      <c r="D56" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E56" s="89">
+      <c r="E56" s="87">
         <v>45436</v>
       </c>
-      <c r="F56" s="88">
-        <v>1</v>
-      </c>
-      <c r="G56" s="91">
+      <c r="F56" s="89">
         <v>45436</v>
       </c>
-      <c r="H56" s="11" t="s">
+      <c r="G56" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H56" s="2"/>
       <c r="I56" s="2"/>
       <c r="J56" s="2"/>
       <c r="K56" s="2"/>
@@ -3964,33 +3832,30 @@
       <c r="S56" s="2"/>
       <c r="T56" s="2"/>
       <c r="U56" s="2"/>
-      <c r="V56" s="2"/>
-    </row>
-    <row r="57" spans="1:168" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="87">
+    </row>
+    <row r="57" spans="1:167" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="85">
         <v>571</v>
       </c>
-      <c r="B57" s="88" t="s">
+      <c r="B57" s="86" t="s">
         <v>232</v>
       </c>
-      <c r="C57" s="88" t="s">
+      <c r="C57" s="86" t="s">
         <v>233</v>
       </c>
-      <c r="D57" s="81" t="s">
+      <c r="D57" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E57" s="89">
+      <c r="E57" s="87">
         <v>45436</v>
       </c>
-      <c r="F57" s="88">
-        <v>1</v>
-      </c>
-      <c r="G57" s="91">
+      <c r="F57" s="89">
         <v>45436</v>
       </c>
-      <c r="H57" s="11" t="s">
+      <c r="G57" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H57" s="10"/>
       <c r="I57" s="10"/>
       <c r="J57" s="10"/>
       <c r="K57" s="10"/>
@@ -4004,33 +3869,30 @@
       <c r="S57" s="10"/>
       <c r="T57" s="10"/>
       <c r="U57" s="10"/>
-      <c r="V57" s="10"/>
-    </row>
-    <row r="58" spans="1:168" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="87">
+    </row>
+    <row r="58" spans="1:167" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="85">
         <v>571</v>
       </c>
-      <c r="B58" s="88" t="s">
+      <c r="B58" s="86" t="s">
         <v>234</v>
       </c>
-      <c r="C58" s="88" t="s">
+      <c r="C58" s="86" t="s">
         <v>235</v>
       </c>
-      <c r="D58" s="81" t="s">
+      <c r="D58" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E58" s="89">
+      <c r="E58" s="87">
         <v>45436</v>
       </c>
-      <c r="F58" s="88">
-        <v>1</v>
-      </c>
-      <c r="G58" s="91">
+      <c r="F58" s="89">
         <v>45436</v>
       </c>
-      <c r="H58" s="11" t="s">
+      <c r="G58" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H58" s="2"/>
       <c r="I58" s="2"/>
       <c r="J58" s="2"/>
       <c r="K58" s="2"/>
@@ -4044,33 +3906,30 @@
       <c r="S58" s="2"/>
       <c r="T58" s="2"/>
       <c r="U58" s="2"/>
-      <c r="V58" s="2"/>
-    </row>
-    <row r="59" spans="1:168" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="87">
+    </row>
+    <row r="59" spans="1:167" s="16" customFormat="1" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="85">
         <v>571</v>
       </c>
-      <c r="B59" s="88" t="s">
+      <c r="B59" s="86" t="s">
         <v>236</v>
       </c>
-      <c r="C59" s="88" t="s">
+      <c r="C59" s="86" t="s">
         <v>237</v>
       </c>
-      <c r="D59" s="81" t="s">
+      <c r="D59" s="79" t="s">
         <v>163</v>
       </c>
-      <c r="E59" s="89">
+      <c r="E59" s="87">
         <v>45436</v>
       </c>
-      <c r="F59" s="88">
-        <v>1</v>
-      </c>
-      <c r="G59" s="91">
+      <c r="F59" s="89">
         <v>45436</v>
       </c>
-      <c r="H59" s="11" t="s">
+      <c r="G59" s="11" t="s">
         <v>48</v>
       </c>
+      <c r="H59" s="2"/>
       <c r="I59" s="2"/>
       <c r="J59" s="2"/>
       <c r="K59" s="2"/>
@@ -4084,31 +3943,30 @@
       <c r="S59" s="2"/>
       <c r="T59" s="2"/>
       <c r="U59" s="2"/>
-      <c r="V59" s="2"/>
-    </row>
-    <row r="60" spans="1:168" s="10" customFormat="1" ht="57" x14ac:dyDescent="0.2">
-      <c r="A60" s="73">
+    </row>
+    <row r="60" spans="1:167" s="10" customFormat="1" ht="38" x14ac:dyDescent="0.2">
+      <c r="A60" s="72">
         <v>581</v>
       </c>
-      <c r="B60" s="73">
+      <c r="B60" s="72">
         <v>628518</v>
       </c>
       <c r="C60" s="69" t="s">
         <v>110</v>
       </c>
-      <c r="D60" s="73" t="s">
+      <c r="D60" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="E60" s="77">
+      <c r="E60" s="76">
         <v>45433</v>
       </c>
-      <c r="F60" s="70"/>
-      <c r="G60" s="77">
+      <c r="F60" s="76">
         <v>45435</v>
       </c>
-      <c r="H60" s="21" t="s">
+      <c r="G60" s="21" t="s">
         <v>50</v>
       </c>
+      <c r="H60" s="2"/>
       <c r="I60" s="2"/>
       <c r="J60" s="2"/>
       <c r="K60" s="2"/>
@@ -4122,7 +3980,7 @@
       <c r="S60" s="2"/>
       <c r="T60" s="2"/>
       <c r="U60" s="2"/>
-      <c r="V60" s="2"/>
+      <c r="V60" s="16"/>
       <c r="W60" s="16"/>
       <c r="X60" s="16"/>
       <c r="Y60" s="16"/>
@@ -4268,31 +4126,30 @@
       <c r="FI60" s="16"/>
       <c r="FJ60" s="16"/>
       <c r="FK60" s="16"/>
-      <c r="FL60" s="16"/>
-    </row>
-    <row r="61" spans="1:168" s="23" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="73">
+    </row>
+    <row r="61" spans="1:167" s="23" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="72">
         <v>381</v>
       </c>
-      <c r="B61" s="73">
+      <c r="B61" s="72">
         <v>592570</v>
       </c>
       <c r="C61" s="69" t="s">
         <v>98</v>
       </c>
-      <c r="D61" s="73" t="s">
+      <c r="D61" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="E61" s="77">
+      <c r="E61" s="76">
         <v>45432</v>
       </c>
-      <c r="F61" s="70"/>
-      <c r="G61" s="77">
+      <c r="F61" s="76">
         <v>45432</v>
       </c>
-      <c r="H61" s="21" t="s">
+      <c r="G61" s="21" t="s">
         <v>50</v>
       </c>
+      <c r="H61" s="2"/>
       <c r="I61" s="2"/>
       <c r="J61" s="2"/>
       <c r="K61" s="2"/>
@@ -4306,7 +4163,7 @@
       <c r="S61" s="2"/>
       <c r="T61" s="2"/>
       <c r="U61" s="2"/>
-      <c r="V61" s="2"/>
+      <c r="V61" s="16"/>
       <c r="W61" s="16"/>
       <c r="X61" s="16"/>
       <c r="Y61" s="16"/>
@@ -4452,31 +4309,30 @@
       <c r="FI61" s="16"/>
       <c r="FJ61" s="16"/>
       <c r="FK61" s="16"/>
-      <c r="FL61" s="16"/>
-    </row>
-    <row r="62" spans="1:168" s="23" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="73">
+    </row>
+    <row r="62" spans="1:167" s="23" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="72">
         <v>481</v>
       </c>
-      <c r="B62" s="73">
+      <c r="B62" s="72">
         <v>581290</v>
       </c>
       <c r="C62" s="69" t="s">
         <v>98</v>
       </c>
-      <c r="D62" s="73" t="s">
+      <c r="D62" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="E62" s="77">
+      <c r="E62" s="76">
         <v>45432</v>
       </c>
-      <c r="F62" s="70"/>
-      <c r="G62" s="77">
+      <c r="F62" s="76">
         <v>45432</v>
       </c>
-      <c r="H62" s="21" t="s">
+      <c r="G62" s="21" t="s">
         <v>50</v>
       </c>
+      <c r="H62" s="2"/>
       <c r="I62" s="2"/>
       <c r="J62" s="2"/>
       <c r="K62" s="2"/>
@@ -4490,7 +4346,7 @@
       <c r="S62" s="2"/>
       <c r="T62" s="2"/>
       <c r="U62" s="2"/>
-      <c r="V62" s="2"/>
+      <c r="V62" s="16"/>
       <c r="W62" s="16"/>
       <c r="X62" s="16"/>
       <c r="Y62" s="16"/>
@@ -4636,31 +4492,30 @@
       <c r="FI62" s="16"/>
       <c r="FJ62" s="16"/>
       <c r="FK62" s="16"/>
-      <c r="FL62" s="16"/>
-    </row>
-    <row r="63" spans="1:168" s="23" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="73">
+    </row>
+    <row r="63" spans="1:167" s="23" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="72">
         <v>391</v>
       </c>
-      <c r="B63" s="72">
+      <c r="B63" s="71">
         <v>593428</v>
       </c>
       <c r="C63" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="D63" s="73" t="s">
+      <c r="D63" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="E63" s="77">
+      <c r="E63" s="76">
         <v>45432</v>
       </c>
-      <c r="F63" s="78"/>
-      <c r="G63" s="77">
+      <c r="F63" s="76">
         <v>45432</v>
       </c>
-      <c r="H63" s="21" t="s">
+      <c r="G63" s="21" t="s">
         <v>50</v>
       </c>
+      <c r="H63" s="2"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
       <c r="K63" s="2"/>
@@ -4674,7 +4529,7 @@
       <c r="S63" s="2"/>
       <c r="T63" s="2"/>
       <c r="U63" s="2"/>
-      <c r="V63" s="2"/>
+      <c r="V63" s="16"/>
       <c r="W63" s="16"/>
       <c r="X63" s="16"/>
       <c r="Y63" s="16"/>
@@ -4820,31 +4675,30 @@
       <c r="FI63" s="16"/>
       <c r="FJ63" s="16"/>
       <c r="FK63" s="16"/>
-      <c r="FL63" s="16"/>
-    </row>
-    <row r="64" spans="1:168" s="23" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="73">
+    </row>
+    <row r="64" spans="1:167" s="23" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="72">
         <v>482</v>
       </c>
-      <c r="B64" s="73">
+      <c r="B64" s="72">
         <v>665882</v>
       </c>
       <c r="C64" s="69" t="s">
         <v>158</v>
       </c>
-      <c r="D64" s="73" t="s">
+      <c r="D64" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="E64" s="77">
+      <c r="E64" s="76">
         <v>45434</v>
       </c>
-      <c r="F64" s="70"/>
-      <c r="G64" s="77">
+      <c r="F64" s="76">
         <v>45434</v>
       </c>
-      <c r="H64" s="21" t="s">
+      <c r="G64" s="21" t="s">
         <v>50</v>
       </c>
+      <c r="H64" s="2"/>
       <c r="I64" s="2"/>
       <c r="J64" s="2"/>
       <c r="K64" s="2"/>
@@ -4858,7 +4712,7 @@
       <c r="S64" s="2"/>
       <c r="T64" s="2"/>
       <c r="U64" s="2"/>
-      <c r="V64" s="2"/>
+      <c r="V64" s="16"/>
       <c r="W64" s="16"/>
       <c r="X64" s="16"/>
       <c r="Y64" s="16"/>
@@ -5004,31 +4858,30 @@
       <c r="FI64" s="16"/>
       <c r="FJ64" s="16"/>
       <c r="FK64" s="16"/>
-      <c r="FL64" s="16"/>
-    </row>
-    <row r="65" spans="1:168" s="23" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="73">
+    </row>
+    <row r="65" spans="1:167" s="23" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="72">
         <v>482</v>
       </c>
-      <c r="B65" s="73">
+      <c r="B65" s="72">
         <v>665877</v>
       </c>
       <c r="C65" s="69" t="s">
         <v>159</v>
       </c>
-      <c r="D65" s="73" t="s">
+      <c r="D65" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="E65" s="77">
+      <c r="E65" s="76">
         <v>45434</v>
       </c>
-      <c r="F65" s="70"/>
-      <c r="G65" s="77">
+      <c r="F65" s="76">
         <v>45434</v>
       </c>
-      <c r="H65" s="21" t="s">
+      <c r="G65" s="21" t="s">
         <v>50</v>
       </c>
+      <c r="H65" s="2"/>
       <c r="I65" s="2"/>
       <c r="J65" s="2"/>
       <c r="K65" s="2"/>
@@ -5042,7 +4895,7 @@
       <c r="S65" s="2"/>
       <c r="T65" s="2"/>
       <c r="U65" s="2"/>
-      <c r="V65" s="2"/>
+      <c r="V65" s="16"/>
       <c r="W65" s="16"/>
       <c r="X65" s="16"/>
       <c r="Y65" s="16"/>
@@ -5188,31 +5041,30 @@
       <c r="FI65" s="16"/>
       <c r="FJ65" s="16"/>
       <c r="FK65" s="16"/>
-      <c r="FL65" s="16"/>
-    </row>
-    <row r="66" spans="1:168" s="23" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="73">
+    </row>
+    <row r="66" spans="1:167" s="23" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="72">
         <v>298</v>
       </c>
-      <c r="B66" s="72">
+      <c r="B66" s="71">
         <v>665169</v>
       </c>
       <c r="C66" s="43" t="s">
         <v>154</v>
       </c>
-      <c r="D66" s="73" t="s">
+      <c r="D66" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="E66" s="77">
+      <c r="E66" s="76">
         <v>45435</v>
       </c>
-      <c r="F66" s="78"/>
-      <c r="G66" s="77">
+      <c r="F66" s="76">
         <v>45435</v>
       </c>
-      <c r="H66" s="21" t="s">
+      <c r="G66" s="21" t="s">
         <v>50</v>
       </c>
+      <c r="H66" s="2"/>
       <c r="I66" s="2"/>
       <c r="J66" s="2"/>
       <c r="K66" s="2"/>
@@ -5226,7 +5078,7 @@
       <c r="S66" s="2"/>
       <c r="T66" s="2"/>
       <c r="U66" s="2"/>
-      <c r="V66" s="2"/>
+      <c r="V66" s="16"/>
       <c r="W66" s="16"/>
       <c r="X66" s="16"/>
       <c r="Y66" s="16"/>
@@ -5372,31 +5224,30 @@
       <c r="FI66" s="16"/>
       <c r="FJ66" s="16"/>
       <c r="FK66" s="16"/>
-      <c r="FL66" s="16"/>
-    </row>
-    <row r="67" spans="1:168" s="23" customFormat="1" ht="38" x14ac:dyDescent="0.2">
-      <c r="A67" s="73">
+    </row>
+    <row r="67" spans="1:167" s="23" customFormat="1" ht="38" x14ac:dyDescent="0.2">
+      <c r="A67" s="72">
         <v>381</v>
       </c>
-      <c r="B67" s="72">
+      <c r="B67" s="71">
         <v>662028</v>
       </c>
       <c r="C67" s="43" t="s">
         <v>160</v>
       </c>
-      <c r="D67" s="73" t="s">
+      <c r="D67" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="E67" s="77">
+      <c r="E67" s="76">
         <v>45435</v>
       </c>
-      <c r="F67" s="78"/>
-      <c r="G67" s="77">
+      <c r="F67" s="76">
         <v>45435</v>
       </c>
-      <c r="H67" s="21" t="s">
+      <c r="G67" s="21" t="s">
         <v>50</v>
       </c>
+      <c r="H67" s="2"/>
       <c r="I67" s="2"/>
       <c r="J67" s="2"/>
       <c r="K67" s="2"/>
@@ -5410,7 +5261,7 @@
       <c r="S67" s="2"/>
       <c r="T67" s="2"/>
       <c r="U67" s="2"/>
-      <c r="V67" s="2"/>
+      <c r="V67" s="16"/>
       <c r="W67" s="16"/>
       <c r="X67" s="16"/>
       <c r="Y67" s="16"/>
@@ -5556,29 +5407,28 @@
       <c r="FI67" s="16"/>
       <c r="FJ67" s="16"/>
       <c r="FK67" s="16"/>
-      <c r="FL67" s="16"/>
-    </row>
-    <row r="68" spans="1:168" s="16" customFormat="1" ht="57" x14ac:dyDescent="0.2">
-      <c r="A68" s="72">
+    </row>
+    <row r="68" spans="1:167" s="16" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="A68" s="71">
         <v>581</v>
       </c>
-      <c r="B68" s="72">
+      <c r="B68" s="71">
         <v>625275</v>
       </c>
       <c r="C68" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="D68" s="72" t="s">
+      <c r="D68" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="E68" s="74" t="s">
+      <c r="E68" s="73" t="s">
         <v>104</v>
       </c>
-      <c r="F68" s="45"/>
-      <c r="G68" s="83"/>
-      <c r="H68" s="11" t="s">
+      <c r="F68" s="81"/>
+      <c r="G68" s="11" t="s">
         <v>240</v>
       </c>
+      <c r="H68" s="2"/>
       <c r="I68" s="2"/>
       <c r="J68" s="2"/>
       <c r="K68" s="2"/>
@@ -5592,31 +5442,30 @@
       <c r="S68" s="2"/>
       <c r="T68" s="2"/>
       <c r="U68" s="2"/>
-      <c r="V68" s="2"/>
-    </row>
-    <row r="69" spans="1:168" s="16" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A69" s="72">
+    </row>
+    <row r="69" spans="1:167" s="16" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A69" s="71">
         <v>381</v>
       </c>
-      <c r="B69" s="72" t="s">
+      <c r="B69" s="71" t="s">
         <v>105</v>
       </c>
       <c r="C69" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="D69" s="72" t="s">
+      <c r="D69" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="E69" s="83">
+      <c r="E69" s="81">
         <v>45430</v>
       </c>
-      <c r="F69" s="45"/>
-      <c r="G69" s="83">
+      <c r="F69" s="81">
         <v>45430</v>
       </c>
-      <c r="H69" s="11" t="s">
+      <c r="G69" s="11" t="s">
         <v>240</v>
       </c>
+      <c r="H69" s="10"/>
       <c r="I69" s="10"/>
       <c r="J69" s="10"/>
       <c r="K69" s="10"/>
@@ -5630,31 +5479,30 @@
       <c r="S69" s="10"/>
       <c r="T69" s="10"/>
       <c r="U69" s="10"/>
-      <c r="V69" s="10"/>
-    </row>
-    <row r="70" spans="1:168" s="16" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A70" s="72">
+    </row>
+    <row r="70" spans="1:167" s="16" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A70" s="71">
         <v>490</v>
       </c>
-      <c r="B70" s="72" t="s">
+      <c r="B70" s="71" t="s">
         <v>150</v>
       </c>
       <c r="C70" s="43" t="s">
         <v>152</v>
       </c>
-      <c r="D70" s="72" t="s">
+      <c r="D70" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="E70" s="74">
+      <c r="E70" s="73">
         <v>45432</v>
       </c>
-      <c r="F70" s="43"/>
-      <c r="G70" s="83">
+      <c r="F70" s="81">
         <v>45432</v>
       </c>
-      <c r="H70" s="11" t="s">
+      <c r="G70" s="11" t="s">
         <v>240</v>
       </c>
+      <c r="H70" s="2"/>
       <c r="I70" s="2"/>
       <c r="J70" s="2"/>
       <c r="K70" s="2"/>
@@ -5668,31 +5516,30 @@
       <c r="S70" s="2"/>
       <c r="T70" s="2"/>
       <c r="U70" s="2"/>
-      <c r="V70" s="2"/>
-    </row>
-    <row r="71" spans="1:168" s="16" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A71" s="72">
+    </row>
+    <row r="71" spans="1:167" s="16" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A71" s="71">
         <v>490</v>
       </c>
-      <c r="B71" s="72" t="s">
+      <c r="B71" s="71" t="s">
         <v>151</v>
       </c>
       <c r="C71" s="43" t="s">
         <v>152</v>
       </c>
-      <c r="D71" s="72" t="s">
+      <c r="D71" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="E71" s="74">
+      <c r="E71" s="73">
         <v>45433</v>
       </c>
-      <c r="F71" s="45"/>
-      <c r="G71" s="83">
+      <c r="F71" s="81">
         <v>45433</v>
       </c>
-      <c r="H71" s="11" t="s">
+      <c r="G71" s="11" t="s">
         <v>240</v>
       </c>
+      <c r="H71" s="10"/>
       <c r="I71" s="10"/>
       <c r="J71" s="10"/>
       <c r="K71" s="10"/>
@@ -5706,31 +5553,30 @@
       <c r="S71" s="10"/>
       <c r="T71" s="10"/>
       <c r="U71" s="10"/>
-      <c r="V71" s="10"/>
-    </row>
-    <row r="72" spans="1:168" s="16" customFormat="1" ht="38" x14ac:dyDescent="0.2">
-      <c r="A72" s="72">
+    </row>
+    <row r="72" spans="1:167" s="16" customFormat="1" ht="38" x14ac:dyDescent="0.2">
+      <c r="A72" s="71">
         <v>298</v>
       </c>
-      <c r="B72" s="72">
+      <c r="B72" s="71">
         <v>659534</v>
       </c>
       <c r="C72" s="43" t="s">
         <v>157</v>
       </c>
-      <c r="D72" s="72" t="s">
+      <c r="D72" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="E72" s="83">
+      <c r="E72" s="81">
         <v>45434</v>
       </c>
-      <c r="F72" s="45"/>
-      <c r="G72" s="83">
+      <c r="F72" s="81">
         <v>45434</v>
       </c>
-      <c r="H72" s="11" t="s">
+      <c r="G72" s="11" t="s">
         <v>240</v>
       </c>
+      <c r="H72" s="2"/>
       <c r="I72" s="2"/>
       <c r="J72" s="2"/>
       <c r="K72" s="2"/>
@@ -5744,31 +5590,30 @@
       <c r="S72" s="2"/>
       <c r="T72" s="2"/>
       <c r="U72" s="2"/>
-      <c r="V72" s="2"/>
-    </row>
-    <row r="73" spans="1:168" s="16" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="72">
+    </row>
+    <row r="73" spans="1:167" s="16" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="71">
         <v>298</v>
       </c>
-      <c r="B73" s="81" t="s">
+      <c r="B73" s="79" t="s">
         <v>155</v>
       </c>
-      <c r="C73" s="82" t="s">
+      <c r="C73" s="80" t="s">
         <v>156</v>
       </c>
-      <c r="D73" s="72" t="s">
+      <c r="D73" s="71" t="s">
         <v>89</v>
       </c>
-      <c r="E73" s="83">
+      <c r="E73" s="81">
         <v>45435</v>
       </c>
-      <c r="F73" s="45"/>
-      <c r="G73" s="83">
+      <c r="F73" s="81">
         <v>45435</v>
       </c>
-      <c r="H73" s="11" t="s">
+      <c r="G73" s="11" t="s">
         <v>240</v>
       </c>
+      <c r="H73" s="2"/>
       <c r="I73" s="2"/>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
@@ -5782,13 +5627,12 @@
       <c r="S73" s="2"/>
       <c r="T73" s="2"/>
       <c r="U73" s="2"/>
-      <c r="V73" s="2"/>
-    </row>
-    <row r="74" spans="1:168" s="16" customFormat="1" ht="38" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="71">
+    </row>
+    <row r="74" spans="1:167" s="16" customFormat="1" ht="38" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="70">
         <v>581</v>
       </c>
-      <c r="B74" s="71">
+      <c r="B74" s="70">
         <v>594901</v>
       </c>
       <c r="C74" s="20" t="s">
@@ -5796,9 +5640,9 @@
       </c>
       <c r="D74" s="24"/>
       <c r="E74" s="52"/>
-      <c r="F74" s="17"/>
-      <c r="G74" s="52"/>
-      <c r="H74" s="11"/>
+      <c r="F74" s="52"/>
+      <c r="G74" s="11"/>
+      <c r="H74" s="10"/>
       <c r="I74" s="10"/>
       <c r="J74" s="10"/>
       <c r="K74" s="10"/>
@@ -5812,17 +5656,16 @@
       <c r="S74" s="10"/>
       <c r="T74" s="10"/>
       <c r="U74" s="10"/>
-      <c r="V74" s="10"/>
-    </row>
-    <row r="75" spans="1:168" s="16" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="71"/>
-      <c r="B75" s="71"/>
+    </row>
+    <row r="75" spans="1:167" s="16" customFormat="1" ht="18" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="70"/>
+      <c r="B75" s="70"/>
       <c r="C75" s="20"/>
       <c r="D75" s="24"/>
       <c r="E75" s="52"/>
-      <c r="F75" s="17"/>
-      <c r="G75" s="52"/>
-      <c r="H75" s="11"/>
+      <c r="F75" s="52"/>
+      <c r="G75" s="11"/>
+      <c r="H75" s="10"/>
       <c r="I75" s="10"/>
       <c r="J75" s="10"/>
       <c r="K75" s="10"/>
@@ -5836,17 +5679,16 @@
       <c r="S75" s="10"/>
       <c r="T75" s="10"/>
       <c r="U75" s="10"/>
-      <c r="V75" s="10"/>
-    </row>
-    <row r="76" spans="1:168" s="10" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="71"/>
-      <c r="B76" s="71"/>
+    </row>
+    <row r="76" spans="1:167" s="10" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="70"/>
+      <c r="B76" s="70"/>
       <c r="C76" s="20"/>
       <c r="D76" s="24"/>
       <c r="E76" s="52"/>
-      <c r="F76" s="17"/>
-      <c r="G76" s="52"/>
-      <c r="H76" s="21"/>
+      <c r="F76" s="52"/>
+      <c r="G76" s="21"/>
+      <c r="H76" s="2"/>
       <c r="I76" s="2"/>
       <c r="J76" s="2"/>
       <c r="K76" s="2"/>
@@ -5860,7 +5702,7 @@
       <c r="S76" s="2"/>
       <c r="T76" s="2"/>
       <c r="U76" s="2"/>
-      <c r="V76" s="2"/>
+      <c r="V76" s="16"/>
       <c r="W76" s="16"/>
       <c r="X76" s="16"/>
       <c r="Y76" s="16"/>
@@ -6006,25 +5848,24 @@
       <c r="FI76" s="16"/>
       <c r="FJ76" s="16"/>
       <c r="FK76" s="16"/>
-      <c r="FL76" s="16"/>
-    </row>
-    <row r="77" spans="1:168" s="16" customFormat="1" ht="57" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="72">
+    </row>
+    <row r="77" spans="1:167" s="16" customFormat="1" ht="57" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="71">
         <v>381</v>
       </c>
-      <c r="B77" s="72">
+      <c r="B77" s="71">
         <v>559093</v>
       </c>
       <c r="C77" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="D77" s="72" t="s">
+      <c r="D77" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E77" s="74"/>
-      <c r="F77" s="45"/>
-      <c r="G77" s="83"/>
-      <c r="H77" s="11"/>
+      <c r="E77" s="73"/>
+      <c r="F77" s="81"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="10"/>
       <c r="I77" s="10"/>
       <c r="J77" s="10"/>
       <c r="K77" s="10"/>
@@ -6038,29 +5879,28 @@
       <c r="S77" s="10"/>
       <c r="T77" s="10"/>
       <c r="U77" s="10"/>
-      <c r="V77" s="10"/>
-    </row>
-    <row r="78" spans="1:168" s="16" customFormat="1" ht="57" x14ac:dyDescent="0.2">
-      <c r="A78" s="72">
+    </row>
+    <row r="78" spans="1:167" s="16" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="A78" s="71">
         <v>391</v>
       </c>
-      <c r="B78" s="72">
+      <c r="B78" s="71">
         <v>642318</v>
       </c>
       <c r="C78" s="43" t="s">
         <v>153</v>
       </c>
-      <c r="D78" s="72" t="s">
+      <c r="D78" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E78" s="74">
+      <c r="E78" s="73">
         <v>45432</v>
       </c>
-      <c r="F78" s="45"/>
-      <c r="G78" s="74"/>
-      <c r="H78" s="11" t="s">
+      <c r="F78" s="73"/>
+      <c r="G78" s="11" t="s">
         <v>239</v>
       </c>
+      <c r="H78" s="2"/>
       <c r="I78" s="2"/>
       <c r="J78" s="2"/>
       <c r="K78" s="2"/>
@@ -6074,29 +5914,28 @@
       <c r="S78" s="2"/>
       <c r="T78" s="2"/>
       <c r="U78" s="2"/>
-      <c r="V78" s="2"/>
-    </row>
-    <row r="79" spans="1:168" s="16" customFormat="1" ht="57" x14ac:dyDescent="0.2">
-      <c r="A79" s="72">
+    </row>
+    <row r="79" spans="1:167" s="16" customFormat="1" ht="57" x14ac:dyDescent="0.2">
+      <c r="A79" s="71">
         <v>391</v>
       </c>
-      <c r="B79" s="72">
+      <c r="B79" s="71">
         <v>637325</v>
       </c>
       <c r="C79" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="D79" s="72" t="s">
+      <c r="D79" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E79" s="83">
+      <c r="E79" s="81">
         <v>45433</v>
       </c>
-      <c r="F79" s="45"/>
-      <c r="G79" s="83"/>
-      <c r="H79" s="11" t="s">
+      <c r="F79" s="81"/>
+      <c r="G79" s="11" t="s">
         <v>239</v>
       </c>
+      <c r="H79" s="2"/>
       <c r="I79" s="2"/>
       <c r="J79" s="2"/>
       <c r="K79" s="2"/>
@@ -6110,31 +5949,30 @@
       <c r="S79" s="2"/>
       <c r="T79" s="2"/>
       <c r="U79" s="2"/>
-      <c r="V79" s="2"/>
-    </row>
-    <row r="80" spans="1:168" s="16" customFormat="1" ht="38" x14ac:dyDescent="0.2">
-      <c r="A80" s="72">
+    </row>
+    <row r="80" spans="1:167" s="16" customFormat="1" ht="38" x14ac:dyDescent="0.2">
+      <c r="A80" s="71">
         <v>391</v>
       </c>
-      <c r="B80" s="72" t="s">
+      <c r="B80" s="71" t="s">
         <v>107</v>
       </c>
       <c r="C80" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="D80" s="72" t="s">
+      <c r="D80" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E80" s="74">
+      <c r="E80" s="73">
         <v>45434</v>
       </c>
-      <c r="F80" s="45"/>
-      <c r="G80" s="74">
+      <c r="F80" s="73">
         <v>45434</v>
       </c>
-      <c r="H80" s="11" t="s">
+      <c r="G80" s="11" t="s">
         <v>239</v>
       </c>
+      <c r="H80" s="2"/>
       <c r="I80" s="2"/>
       <c r="J80" s="2"/>
       <c r="K80" s="2"/>
@@ -6148,31 +5986,30 @@
       <c r="S80" s="2"/>
       <c r="T80" s="2"/>
       <c r="U80" s="2"/>
-      <c r="V80" s="2"/>
-    </row>
-    <row r="81" spans="1:22" s="16" customFormat="1" ht="38" x14ac:dyDescent="0.2">
-      <c r="A81" s="72">
+    </row>
+    <row r="81" spans="1:21" s="16" customFormat="1" ht="38" x14ac:dyDescent="0.2">
+      <c r="A81" s="71">
         <v>581</v>
       </c>
-      <c r="B81" s="72">
+      <c r="B81" s="71">
         <v>662524</v>
       </c>
       <c r="C81" s="43" t="s">
         <v>149</v>
       </c>
-      <c r="D81" s="72" t="s">
+      <c r="D81" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="E81" s="74">
+      <c r="E81" s="73">
         <v>45435</v>
       </c>
-      <c r="F81" s="45"/>
-      <c r="G81" s="74">
+      <c r="F81" s="73">
         <v>45435</v>
       </c>
-      <c r="H81" s="11" t="s">
+      <c r="G81" s="11" t="s">
         <v>239</v>
       </c>
+      <c r="H81" s="10"/>
       <c r="I81" s="10"/>
       <c r="J81" s="10"/>
       <c r="K81" s="10"/>
@@ -6186,7 +6023,6 @@
       <c r="S81" s="10"/>
       <c r="T81" s="10"/>
       <c r="U81" s="10"/>
-      <c r="V81" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
@@ -6225,34 +6061,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="101" t="s">
+      <c r="A1" s="99" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="101"/>
-      <c r="C1" s="101"/>
-      <c r="D1" s="101"/>
-      <c r="E1" s="101"/>
-      <c r="F1" s="101"/>
-      <c r="G1" s="101"/>
-      <c r="H1" s="101"/>
-      <c r="I1" s="101"/>
-      <c r="J1" s="101"/>
-      <c r="K1" s="101"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="99"/>
+      <c r="G1" s="99"/>
+      <c r="H1" s="99"/>
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
-      <c r="E2" s="102"/>
-      <c r="F2" s="102"/>
-      <c r="G2" s="102"/>
-      <c r="H2" s="102"/>
-      <c r="I2" s="102"/>
-      <c r="J2" s="102"/>
-      <c r="K2" s="102"/>
+      <c r="B2" s="100"/>
+      <c r="C2" s="100"/>
+      <c r="D2" s="100"/>
+      <c r="E2" s="100"/>
+      <c r="F2" s="100"/>
+      <c r="G2" s="100"/>
+      <c r="H2" s="100"/>
+      <c r="I2" s="100"/>
+      <c r="J2" s="100"/>
+      <c r="K2" s="100"/>
     </row>
     <row r="3" spans="1:11" s="10" customFormat="1" ht="57" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
@@ -6290,19 +6126,19 @@
       </c>
     </row>
     <row r="4" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="96">
+      <c r="A4" s="94">
         <v>391</v>
       </c>
-      <c r="B4" s="99"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
-      <c r="H4" s="99"/>
-      <c r="I4" s="99"/>
-      <c r="J4" s="99"/>
-      <c r="K4" s="100"/>
+      <c r="B4" s="97"/>
+      <c r="C4" s="97"/>
+      <c r="D4" s="97"/>
+      <c r="E4" s="97"/>
+      <c r="F4" s="97"/>
+      <c r="G4" s="97"/>
+      <c r="H4" s="97"/>
+      <c r="I4" s="97"/>
+      <c r="J4" s="97"/>
+      <c r="K4" s="98"/>
     </row>
     <row r="5" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="20"/>
@@ -6499,19 +6335,19 @@
       <c r="K19" s="18"/>
     </row>
     <row r="20" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="96" t="s">
+      <c r="A20" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="99"/>
-      <c r="C20" s="99"/>
-      <c r="D20" s="99"/>
-      <c r="E20" s="99"/>
-      <c r="F20" s="99"/>
-      <c r="G20" s="99"/>
-      <c r="H20" s="99"/>
-      <c r="I20" s="99"/>
-      <c r="J20" s="99"/>
-      <c r="K20" s="100"/>
+      <c r="B20" s="97"/>
+      <c r="C20" s="97"/>
+      <c r="D20" s="97"/>
+      <c r="E20" s="97"/>
+      <c r="F20" s="97"/>
+      <c r="G20" s="97"/>
+      <c r="H20" s="97"/>
+      <c r="I20" s="97"/>
+      <c r="J20" s="97"/>
+      <c r="K20" s="98"/>
     </row>
     <row r="21" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="20"/>
@@ -6644,19 +6480,19 @@
       <c r="K30" s="25"/>
     </row>
     <row r="31" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="96" t="s">
+      <c r="A31" s="94" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="103"/>
-      <c r="C31" s="103"/>
-      <c r="D31" s="103"/>
-      <c r="E31" s="103"/>
-      <c r="F31" s="103"/>
-      <c r="G31" s="103"/>
-      <c r="H31" s="103"/>
-      <c r="I31" s="103"/>
-      <c r="J31" s="103"/>
-      <c r="K31" s="104"/>
+      <c r="B31" s="101"/>
+      <c r="C31" s="101"/>
+      <c r="D31" s="101"/>
+      <c r="E31" s="101"/>
+      <c r="F31" s="101"/>
+      <c r="G31" s="101"/>
+      <c r="H31" s="101"/>
+      <c r="I31" s="101"/>
+      <c r="J31" s="101"/>
+      <c r="K31" s="102"/>
     </row>
     <row r="32" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="20"/>
@@ -6750,19 +6586,19 @@
       <c r="K38" s="20"/>
     </row>
     <row r="39" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="96" t="s">
+      <c r="A39" s="94" t="s">
         <v>10</v>
       </c>
-      <c r="B39" s="105"/>
-      <c r="C39" s="105"/>
-      <c r="D39" s="105"/>
-      <c r="E39" s="105"/>
-      <c r="F39" s="105"/>
-      <c r="G39" s="105"/>
-      <c r="H39" s="105"/>
-      <c r="I39" s="105"/>
-      <c r="J39" s="105"/>
-      <c r="K39" s="106"/>
+      <c r="B39" s="103"/>
+      <c r="C39" s="103"/>
+      <c r="D39" s="103"/>
+      <c r="E39" s="103"/>
+      <c r="F39" s="103"/>
+      <c r="G39" s="103"/>
+      <c r="H39" s="103"/>
+      <c r="I39" s="103"/>
+      <c r="J39" s="103"/>
+      <c r="K39" s="104"/>
     </row>
     <row r="40" spans="1:11" s="10" customFormat="1" ht="19" x14ac:dyDescent="0.2">
       <c r="A40" s="20">
@@ -6841,19 +6677,19 @@
       <c r="K43" s="25"/>
     </row>
     <row r="44" spans="1:11" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="96" t="s">
+      <c r="A44" s="94" t="s">
         <v>11</v>
       </c>
-      <c r="B44" s="105"/>
-      <c r="C44" s="105"/>
-      <c r="D44" s="105"/>
-      <c r="E44" s="105"/>
-      <c r="F44" s="105"/>
-      <c r="G44" s="105"/>
-      <c r="H44" s="105"/>
-      <c r="I44" s="105"/>
-      <c r="J44" s="105"/>
-      <c r="K44" s="106"/>
+      <c r="B44" s="103"/>
+      <c r="C44" s="103"/>
+      <c r="D44" s="103"/>
+      <c r="E44" s="103"/>
+      <c r="F44" s="103"/>
+      <c r="G44" s="103"/>
+      <c r="H44" s="103"/>
+      <c r="I44" s="103"/>
+      <c r="J44" s="103"/>
+      <c r="K44" s="104"/>
     </row>
     <row r="45" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="36"/>
@@ -6907,19 +6743,19 @@
       <c r="K48" s="25"/>
     </row>
     <row r="49" spans="1:11" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="96" t="s">
+      <c r="A49" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="B49" s="97"/>
-      <c r="C49" s="97"/>
-      <c r="D49" s="97"/>
-      <c r="E49" s="97"/>
-      <c r="F49" s="97"/>
-      <c r="G49" s="97"/>
-      <c r="H49" s="97"/>
-      <c r="I49" s="97"/>
-      <c r="J49" s="97"/>
-      <c r="K49" s="98"/>
+      <c r="B49" s="95"/>
+      <c r="C49" s="95"/>
+      <c r="D49" s="95"/>
+      <c r="E49" s="95"/>
+      <c r="F49" s="95"/>
+      <c r="G49" s="95"/>
+      <c r="H49" s="95"/>
+      <c r="I49" s="95"/>
+      <c r="J49" s="95"/>
+      <c r="K49" s="96"/>
     </row>
     <row r="50" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="20"/>
@@ -7026,17 +6862,17 @@
       <c r="K57" s="26"/>
     </row>
     <row r="58" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="96"/>
-      <c r="B58" s="97"/>
-      <c r="C58" s="97"/>
-      <c r="D58" s="97"/>
-      <c r="E58" s="97"/>
-      <c r="F58" s="97"/>
-      <c r="G58" s="97"/>
-      <c r="H58" s="97"/>
-      <c r="I58" s="97"/>
-      <c r="J58" s="97"/>
-      <c r="K58" s="98"/>
+      <c r="A58" s="94"/>
+      <c r="B58" s="95"/>
+      <c r="C58" s="95"/>
+      <c r="D58" s="95"/>
+      <c r="E58" s="95"/>
+      <c r="F58" s="95"/>
+      <c r="G58" s="95"/>
+      <c r="H58" s="95"/>
+      <c r="I58" s="95"/>
+      <c r="J58" s="95"/>
+      <c r="K58" s="96"/>
     </row>
     <row r="59" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="26"/>
@@ -8809,6 +8645,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002DF2C0C409D15846B22A3E28E5C3867E" ma:contentTypeVersion="7" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="48ab47e84bb093800bf9be23da141eef">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="39d22158-14c6-450f-a1b3-cc39ff917f42" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eb0f9c9e744cd71b9a78bb2cf2db3121" ns3:_="">
     <xsd:import namespace="39d22158-14c6-450f-a1b3-cc39ff917f42"/>
@@ -8972,22 +8823,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{041E51C1-5B76-4988-B627-C0AD68B41A29}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="39d22158-14c6-450f-a1b3-cc39ff917f42"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82017AFD-1C83-4612-AC65-AE984A1CC780}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AEEBC474-4D4A-43AD-96E8-D62233B3988C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9003,28 +8863,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{82017AFD-1C83-4612-AC65-AE984A1CC780}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{041E51C1-5B76-4988-B627-C0AD68B41A29}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="39d22158-14c6-450f-a1b3-cc39ff917f42"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>